<commit_message>
treinando o naive bayes
</commit_message>
<xml_diff>
--- a/portugues/pt_troubleshooting.xlsx
+++ b/portugues/pt_troubleshooting.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\chatbot_hipotese\portugues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9239B10-A715-41E0-AC23-27CBE0B248D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EECE59-B4DC-4BC4-8B0A-ECC4A618CFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pt" sheetId="1" r:id="rId1"/>
     <sheet name="en" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pt!$A$1:$G$523</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3692,10 +3695,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H523"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D224" sqref="D224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3730,7 +3734,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3756,7 +3760,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -3783,7 +3787,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
@@ -3810,7 +3814,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3837,7 +3841,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3864,7 +3868,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3891,7 +3895,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3918,7 +3922,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3945,7 +3949,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3972,7 +3976,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3999,7 +4003,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4023,7 +4027,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4050,7 +4054,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4077,7 +4081,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4104,7 +4108,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4131,7 +4135,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4158,7 +4162,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4185,7 +4189,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4212,7 +4216,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4239,7 +4243,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4266,7 +4270,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4293,7 +4297,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4320,7 +4324,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4347,7 +4351,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4374,7 +4378,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4401,7 +4405,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4428,7 +4432,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4455,7 +4459,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4482,7 +4486,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4509,7 +4513,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4536,7 +4540,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4563,7 +4567,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4590,7 +4594,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4617,7 +4621,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -4644,7 +4648,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -4671,7 +4675,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -4698,7 +4702,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -4725,7 +4729,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -4752,7 +4756,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -4779,7 +4783,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -4806,7 +4810,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -4833,7 +4837,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -4860,7 +4864,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -4887,7 +4891,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -4914,7 +4918,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -4941,7 +4945,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -4968,7 +4972,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -4995,7 +4999,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -5022,7 +5026,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -5049,7 +5053,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -5076,7 +5080,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -5103,7 +5107,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -5130,7 +5134,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -5157,7 +5161,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -5184,7 +5188,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -5211,7 +5215,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -5238,7 +5242,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -5265,7 +5269,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -5292,7 +5296,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -5319,7 +5323,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -5346,7 +5350,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -5373,7 +5377,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -5400,7 +5404,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -5427,7 +5431,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -5454,7 +5458,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -5481,7 +5485,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -5508,7 +5512,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" ref="A68:A131" si="1">A67+1</f>
         <v>66</v>
@@ -5535,7 +5539,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -5562,7 +5566,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -5589,7 +5593,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -5616,7 +5620,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -5643,7 +5647,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -5670,7 +5674,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -5697,7 +5701,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -5724,7 +5728,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -5751,7 +5755,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -5778,7 +5782,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -5805,7 +5809,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -5832,7 +5836,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -5859,7 +5863,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -5886,7 +5890,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -5913,7 +5917,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -5940,7 +5944,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -5967,7 +5971,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -5994,7 +5998,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -6021,7 +6025,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -6048,7 +6052,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -6075,7 +6079,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -6102,7 +6106,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -6129,7 +6133,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -6156,7 +6160,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -6183,7 +6187,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -6210,7 +6214,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -6237,7 +6241,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -6264,7 +6268,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -6291,7 +6295,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -6318,7 +6322,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -6345,7 +6349,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -6372,7 +6376,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -6399,7 +6403,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -6426,7 +6430,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -6453,7 +6457,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -6480,7 +6484,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -6507,7 +6511,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -6534,7 +6538,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -6561,7 +6565,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -6588,7 +6592,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -6615,7 +6619,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -6642,7 +6646,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -6669,7 +6673,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -6696,7 +6700,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -6723,7 +6727,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -6750,7 +6754,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -6777,7 +6781,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -6804,7 +6808,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -6831,7 +6835,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -6858,7 +6862,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -6885,7 +6889,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -6912,7 +6916,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -6939,7 +6943,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -6966,7 +6970,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -6993,7 +6997,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -7020,7 +7024,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -7047,7 +7051,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -7074,7 +7078,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -7101,7 +7105,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -7128,7 +7132,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -7155,7 +7159,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -7182,7 +7186,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <f t="shared" si="1"/>
         <v>128</v>
@@ -7209,7 +7213,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -7236,7 +7240,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <f t="shared" ref="A132:A195" si="2">A131+1</f>
         <v>130</v>
@@ -7263,7 +7267,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <f t="shared" si="2"/>
         <v>131</v>
@@ -7290,7 +7294,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <f t="shared" si="2"/>
         <v>132</v>
@@ -7317,7 +7321,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <f t="shared" si="2"/>
         <v>133</v>
@@ -7344,7 +7348,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <f t="shared" si="2"/>
         <v>134</v>
@@ -7371,7 +7375,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <f t="shared" si="2"/>
         <v>135</v>
@@ -7398,7 +7402,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <f t="shared" si="2"/>
         <v>136</v>
@@ -7425,7 +7429,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <f t="shared" si="2"/>
         <v>137</v>
@@ -7452,7 +7456,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <f t="shared" si="2"/>
         <v>138</v>
@@ -7479,7 +7483,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -7506,7 +7510,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -7533,7 +7537,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -7560,7 +7564,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -7587,7 +7591,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -7614,7 +7618,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -7641,7 +7645,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -7668,7 +7672,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -7695,7 +7699,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -7722,7 +7726,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -7749,7 +7753,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -7776,7 +7780,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -7803,7 +7807,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -7830,7 +7834,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -7857,7 +7861,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -7884,7 +7888,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -7911,7 +7915,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <f t="shared" si="2"/>
         <v>155</v>
@@ -7938,7 +7942,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <f t="shared" si="2"/>
         <v>156</v>
@@ -7965,7 +7969,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <f t="shared" si="2"/>
         <v>157</v>
@@ -7992,7 +7996,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <f t="shared" si="2"/>
         <v>158</v>
@@ -8019,7 +8023,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <f t="shared" si="2"/>
         <v>159</v>
@@ -8046,7 +8050,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <f t="shared" si="2"/>
         <v>160</v>
@@ -8073,7 +8077,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <f t="shared" si="2"/>
         <v>161</v>
@@ -8100,7 +8104,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <f t="shared" si="2"/>
         <v>162</v>
@@ -8127,7 +8131,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <f t="shared" si="2"/>
         <v>163</v>
@@ -8154,7 +8158,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <f t="shared" si="2"/>
         <v>164</v>
@@ -8181,7 +8185,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <f t="shared" si="2"/>
         <v>165</v>
@@ -8208,7 +8212,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <f t="shared" si="2"/>
         <v>166</v>
@@ -8235,7 +8239,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <f t="shared" si="2"/>
         <v>167</v>
@@ -8262,7 +8266,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <f t="shared" si="2"/>
         <v>168</v>
@@ -8289,7 +8293,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <f t="shared" si="2"/>
         <v>169</v>
@@ -8316,7 +8320,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <f t="shared" si="2"/>
         <v>170</v>
@@ -8343,7 +8347,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <f t="shared" si="2"/>
         <v>171</v>
@@ -8370,7 +8374,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <f t="shared" si="2"/>
         <v>172</v>
@@ -8397,7 +8401,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <f t="shared" si="2"/>
         <v>173</v>
@@ -8424,7 +8428,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <f t="shared" si="2"/>
         <v>174</v>
@@ -8451,7 +8455,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <f t="shared" si="2"/>
         <v>175</v>
@@ -8478,7 +8482,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <f t="shared" si="2"/>
         <v>176</v>
@@ -8505,7 +8509,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <f t="shared" si="2"/>
         <v>177</v>
@@ -8532,7 +8536,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <f t="shared" si="2"/>
         <v>178</v>
@@ -8559,7 +8563,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <f t="shared" si="2"/>
         <v>179</v>
@@ -8586,7 +8590,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <f t="shared" si="2"/>
         <v>180</v>
@@ -8613,7 +8617,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <f t="shared" si="2"/>
         <v>181</v>
@@ -8640,7 +8644,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <f t="shared" si="2"/>
         <v>182</v>
@@ -8667,7 +8671,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <f t="shared" si="2"/>
         <v>183</v>
@@ -8694,7 +8698,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <f t="shared" si="2"/>
         <v>184</v>
@@ -8721,7 +8725,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <f t="shared" si="2"/>
         <v>185</v>
@@ -8748,7 +8752,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <f t="shared" si="2"/>
         <v>186</v>
@@ -8775,7 +8779,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <f t="shared" si="2"/>
         <v>187</v>
@@ -8802,7 +8806,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <f t="shared" si="2"/>
         <v>188</v>
@@ -8829,7 +8833,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <f t="shared" si="2"/>
         <v>189</v>
@@ -8856,7 +8860,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <f t="shared" si="2"/>
         <v>190</v>
@@ -8883,7 +8887,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <f t="shared" si="2"/>
         <v>191</v>
@@ -8910,7 +8914,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <f t="shared" si="2"/>
         <v>192</v>
@@ -8934,7 +8938,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <f t="shared" si="2"/>
         <v>193</v>
@@ -8961,7 +8965,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <f t="shared" ref="A196:A259" si="3">A195+1</f>
         <v>194</v>
@@ -8988,7 +8992,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <f t="shared" si="3"/>
         <v>195</v>
@@ -9015,7 +9019,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <f t="shared" si="3"/>
         <v>196</v>
@@ -9042,7 +9046,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <f t="shared" si="3"/>
         <v>197</v>
@@ -9069,7 +9073,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <f t="shared" si="3"/>
         <v>198</v>
@@ -9096,7 +9100,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <f t="shared" si="3"/>
         <v>199</v>
@@ -9123,7 +9127,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <f t="shared" si="3"/>
         <v>200</v>
@@ -9150,7 +9154,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <f t="shared" si="3"/>
         <v>201</v>
@@ -9177,7 +9181,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <f t="shared" si="3"/>
         <v>202</v>
@@ -9204,7 +9208,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <f t="shared" si="3"/>
         <v>203</v>
@@ -9231,7 +9235,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <f t="shared" si="3"/>
         <v>204</v>
@@ -9258,7 +9262,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <f t="shared" si="3"/>
         <v>205</v>
@@ -9285,7 +9289,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <f t="shared" si="3"/>
         <v>206</v>
@@ -9312,7 +9316,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <f t="shared" si="3"/>
         <v>207</v>
@@ -9339,7 +9343,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <f t="shared" si="3"/>
         <v>208</v>
@@ -9366,7 +9370,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <f t="shared" si="3"/>
         <v>209</v>
@@ -9393,7 +9397,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <f t="shared" si="3"/>
         <v>210</v>
@@ -9420,7 +9424,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <f t="shared" si="3"/>
         <v>211</v>
@@ -9447,7 +9451,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <f t="shared" si="3"/>
         <v>212</v>
@@ -9474,7 +9478,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <f t="shared" si="3"/>
         <v>213</v>
@@ -9501,7 +9505,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <f t="shared" si="3"/>
         <v>214</v>
@@ -9528,7 +9532,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <f t="shared" si="3"/>
         <v>215</v>
@@ -9555,7 +9559,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <f t="shared" si="3"/>
         <v>216</v>
@@ -9582,7 +9586,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <f t="shared" si="3"/>
         <v>217</v>
@@ -9609,7 +9613,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <f t="shared" si="3"/>
         <v>218</v>
@@ -9636,7 +9640,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <f t="shared" si="3"/>
         <v>219</v>
@@ -9663,7 +9667,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <f t="shared" si="3"/>
         <v>220</v>
@@ -9690,7 +9694,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <f t="shared" si="3"/>
         <v>221</v>
@@ -10365,7 +10369,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <f t="shared" si="3"/>
         <v>246</v>
@@ -10392,7 +10396,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <f t="shared" si="3"/>
         <v>247</v>
@@ -10419,7 +10423,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <f t="shared" si="3"/>
         <v>248</v>
@@ -10446,7 +10450,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <f t="shared" si="3"/>
         <v>249</v>
@@ -10473,7 +10477,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <f t="shared" si="3"/>
         <v>250</v>
@@ -10500,7 +10504,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <f t="shared" si="3"/>
         <v>251</v>
@@ -10527,7 +10531,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <f t="shared" si="3"/>
         <v>252</v>
@@ -10554,7 +10558,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <f t="shared" si="3"/>
         <v>253</v>
@@ -10581,7 +10585,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <f t="shared" si="3"/>
         <v>254</v>
@@ -10608,7 +10612,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <f t="shared" si="3"/>
         <v>255</v>
@@ -10635,7 +10639,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <f t="shared" si="3"/>
         <v>256</v>
@@ -10662,7 +10666,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <f t="shared" si="3"/>
         <v>257</v>
@@ -10689,7 +10693,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <f t="shared" ref="A260:A323" si="4">A259+1</f>
         <v>258</v>
@@ -10716,7 +10720,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <f t="shared" si="4"/>
         <v>259</v>
@@ -10743,7 +10747,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <f t="shared" si="4"/>
         <v>260</v>
@@ -10770,7 +10774,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <f t="shared" si="4"/>
         <v>261</v>
@@ -10797,7 +10801,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <f t="shared" si="4"/>
         <v>262</v>
@@ -10824,7 +10828,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <f t="shared" si="4"/>
         <v>263</v>
@@ -10851,7 +10855,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <f t="shared" si="4"/>
         <v>264</v>
@@ -10878,7 +10882,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <f t="shared" si="4"/>
         <v>265</v>
@@ -10905,7 +10909,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <f t="shared" si="4"/>
         <v>266</v>
@@ -10932,7 +10936,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <f t="shared" si="4"/>
         <v>267</v>
@@ -10959,7 +10963,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <f t="shared" si="4"/>
         <v>268</v>
@@ -10986,7 +10990,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <f t="shared" si="4"/>
         <v>269</v>
@@ -11013,7 +11017,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <f t="shared" si="4"/>
         <v>270</v>
@@ -11040,7 +11044,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <f t="shared" si="4"/>
         <v>271</v>
@@ -11067,7 +11071,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <f t="shared" si="4"/>
         <v>272</v>
@@ -11094,7 +11098,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <f t="shared" si="4"/>
         <v>273</v>
@@ -11121,7 +11125,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <f t="shared" si="4"/>
         <v>274</v>
@@ -11148,7 +11152,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <f t="shared" si="4"/>
         <v>275</v>
@@ -11175,7 +11179,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <f t="shared" si="4"/>
         <v>276</v>
@@ -11202,7 +11206,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <f t="shared" si="4"/>
         <v>277</v>
@@ -11229,7 +11233,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <f t="shared" si="4"/>
         <v>278</v>
@@ -11256,7 +11260,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <f t="shared" si="4"/>
         <v>279</v>
@@ -11283,7 +11287,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <f t="shared" si="4"/>
         <v>280</v>
@@ -11310,7 +11314,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <f t="shared" si="4"/>
         <v>281</v>
@@ -11337,7 +11341,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <f t="shared" si="4"/>
         <v>282</v>
@@ -11364,7 +11368,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <f t="shared" si="4"/>
         <v>283</v>
@@ -11391,7 +11395,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <f t="shared" si="4"/>
         <v>284</v>
@@ -11418,7 +11422,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <f t="shared" si="4"/>
         <v>285</v>
@@ -11445,7 +11449,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <f t="shared" si="4"/>
         <v>286</v>
@@ -11472,7 +11476,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <f t="shared" si="4"/>
         <v>287</v>
@@ -11499,7 +11503,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <f t="shared" si="4"/>
         <v>288</v>
@@ -11526,7 +11530,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <f t="shared" si="4"/>
         <v>289</v>
@@ -11553,7 +11557,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <f t="shared" si="4"/>
         <v>290</v>
@@ -11580,7 +11584,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <f t="shared" si="4"/>
         <v>291</v>
@@ -11607,7 +11611,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <f t="shared" si="4"/>
         <v>292</v>
@@ -11634,7 +11638,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <f t="shared" si="4"/>
         <v>293</v>
@@ -11661,7 +11665,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <f t="shared" si="4"/>
         <v>294</v>
@@ -11688,7 +11692,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <f t="shared" si="4"/>
         <v>295</v>
@@ -11715,7 +11719,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <f t="shared" si="4"/>
         <v>296</v>
@@ -11742,7 +11746,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <f t="shared" si="4"/>
         <v>297</v>
@@ -11769,7 +11773,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <f t="shared" si="4"/>
         <v>298</v>
@@ -11796,7 +11800,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <f t="shared" si="4"/>
         <v>299</v>
@@ -11823,7 +11827,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <f t="shared" si="4"/>
         <v>300</v>
@@ -11850,7 +11854,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <f t="shared" si="4"/>
         <v>301</v>
@@ -11877,7 +11881,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <f t="shared" si="4"/>
         <v>302</v>
@@ -11901,7 +11905,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <f t="shared" si="4"/>
         <v>303</v>
@@ -11925,7 +11929,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <f t="shared" si="4"/>
         <v>304</v>
@@ -11952,7 +11956,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <f t="shared" si="4"/>
         <v>305</v>
@@ -11979,7 +11983,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <f t="shared" si="4"/>
         <v>306</v>
@@ -12006,7 +12010,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <f t="shared" si="4"/>
         <v>307</v>
@@ -12033,7 +12037,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <f t="shared" si="4"/>
         <v>308</v>
@@ -12060,7 +12064,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <f t="shared" si="4"/>
         <v>309</v>
@@ -12087,7 +12091,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <f t="shared" si="4"/>
         <v>310</v>
@@ -12114,7 +12118,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <f t="shared" si="4"/>
         <v>311</v>
@@ -12141,7 +12145,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <f t="shared" si="4"/>
         <v>312</v>
@@ -12168,7 +12172,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <f t="shared" si="4"/>
         <v>313</v>
@@ -12195,7 +12199,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <f t="shared" si="4"/>
         <v>314</v>
@@ -12222,7 +12226,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <f t="shared" si="4"/>
         <v>315</v>
@@ -12249,7 +12253,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <f t="shared" si="4"/>
         <v>316</v>
@@ -12276,7 +12280,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <f t="shared" si="4"/>
         <v>317</v>
@@ -12303,7 +12307,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <f t="shared" si="4"/>
         <v>318</v>
@@ -12330,7 +12334,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <f t="shared" si="4"/>
         <v>319</v>
@@ -12357,7 +12361,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <f t="shared" si="4"/>
         <v>320</v>
@@ -12384,7 +12388,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <f t="shared" si="4"/>
         <v>321</v>
@@ -12411,7 +12415,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <f t="shared" ref="A324:A387" si="5">A323+1</f>
         <v>322</v>
@@ -12438,7 +12442,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <f t="shared" si="5"/>
         <v>323</v>
@@ -12465,7 +12469,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <f t="shared" si="5"/>
         <v>324</v>
@@ -12492,7 +12496,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <f t="shared" si="5"/>
         <v>325</v>
@@ -12519,7 +12523,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <f t="shared" si="5"/>
         <v>326</v>
@@ -12546,7 +12550,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <f t="shared" si="5"/>
         <v>327</v>
@@ -12573,7 +12577,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <f t="shared" si="5"/>
         <v>328</v>
@@ -12600,7 +12604,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <f t="shared" si="5"/>
         <v>329</v>
@@ -12627,7 +12631,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <f t="shared" si="5"/>
         <v>330</v>
@@ -12654,7 +12658,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <f t="shared" si="5"/>
         <v>331</v>
@@ -12681,7 +12685,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <f t="shared" si="5"/>
         <v>332</v>
@@ -12708,7 +12712,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <f t="shared" si="5"/>
         <v>333</v>
@@ -12735,7 +12739,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <f t="shared" si="5"/>
         <v>334</v>
@@ -12762,7 +12766,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <f t="shared" si="5"/>
         <v>335</v>
@@ -12789,7 +12793,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <f t="shared" si="5"/>
         <v>336</v>
@@ -12816,7 +12820,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <f t="shared" si="5"/>
         <v>337</v>
@@ -12843,7 +12847,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <f t="shared" si="5"/>
         <v>338</v>
@@ -12870,7 +12874,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <f t="shared" si="5"/>
         <v>339</v>
@@ -12897,7 +12901,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <f t="shared" si="5"/>
         <v>340</v>
@@ -12924,7 +12928,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <f t="shared" si="5"/>
         <v>341</v>
@@ -12951,7 +12955,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <f t="shared" si="5"/>
         <v>342</v>
@@ -12978,7 +12982,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <f t="shared" si="5"/>
         <v>343</v>
@@ -13005,7 +13009,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <f t="shared" si="5"/>
         <v>344</v>
@@ -13032,7 +13036,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <f t="shared" si="5"/>
         <v>345</v>
@@ -13059,7 +13063,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <f t="shared" si="5"/>
         <v>346</v>
@@ -13086,7 +13090,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <f t="shared" si="5"/>
         <v>347</v>
@@ -13113,7 +13117,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <f t="shared" si="5"/>
         <v>348</v>
@@ -13140,7 +13144,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <f t="shared" si="5"/>
         <v>349</v>
@@ -13167,7 +13171,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <f t="shared" si="5"/>
         <v>350</v>
@@ -13194,7 +13198,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <f t="shared" si="5"/>
         <v>351</v>
@@ -13221,7 +13225,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <f t="shared" si="5"/>
         <v>352</v>
@@ -13248,7 +13252,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <f t="shared" si="5"/>
         <v>353</v>
@@ -13275,7 +13279,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <f t="shared" si="5"/>
         <v>354</v>
@@ -13302,7 +13306,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <f t="shared" si="5"/>
         <v>355</v>
@@ -13329,7 +13333,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <f t="shared" si="5"/>
         <v>356</v>
@@ -13356,7 +13360,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <f t="shared" si="5"/>
         <v>357</v>
@@ -13383,7 +13387,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <f t="shared" si="5"/>
         <v>358</v>
@@ -13410,7 +13414,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <f t="shared" si="5"/>
         <v>359</v>
@@ -13437,7 +13441,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <f t="shared" si="5"/>
         <v>360</v>
@@ -13464,7 +13468,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <f t="shared" si="5"/>
         <v>361</v>
@@ -13491,7 +13495,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <f t="shared" si="5"/>
         <v>362</v>
@@ -13518,7 +13522,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <f t="shared" si="5"/>
         <v>363</v>
@@ -13545,7 +13549,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <f t="shared" si="5"/>
         <v>364</v>
@@ -13572,7 +13576,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <f t="shared" si="5"/>
         <v>365</v>
@@ -13599,7 +13603,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <f t="shared" si="5"/>
         <v>366</v>
@@ -13626,7 +13630,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <f t="shared" si="5"/>
         <v>367</v>
@@ -13653,7 +13657,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <f t="shared" si="5"/>
         <v>368</v>
@@ -13680,7 +13684,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <f t="shared" si="5"/>
         <v>369</v>
@@ -13707,7 +13711,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <f t="shared" si="5"/>
         <v>370</v>
@@ -13734,7 +13738,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <f t="shared" si="5"/>
         <v>371</v>
@@ -13761,7 +13765,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <f t="shared" si="5"/>
         <v>372</v>
@@ -13788,7 +13792,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <f t="shared" si="5"/>
         <v>373</v>
@@ -13815,7 +13819,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <f t="shared" si="5"/>
         <v>374</v>
@@ -13842,7 +13846,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <f t="shared" si="5"/>
         <v>375</v>
@@ -13869,7 +13873,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <f t="shared" si="5"/>
         <v>376</v>
@@ -13896,7 +13900,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <f t="shared" si="5"/>
         <v>377</v>
@@ -13923,7 +13927,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <f t="shared" si="5"/>
         <v>378</v>
@@ -13950,7 +13954,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <f t="shared" si="5"/>
         <v>379</v>
@@ -13977,7 +13981,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <f t="shared" si="5"/>
         <v>380</v>
@@ -14004,7 +14008,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <f t="shared" si="5"/>
         <v>381</v>
@@ -14031,7 +14035,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <f t="shared" si="5"/>
         <v>382</v>
@@ -14058,7 +14062,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <f t="shared" si="5"/>
         <v>383</v>
@@ -14085,7 +14089,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <f t="shared" si="5"/>
         <v>384</v>
@@ -14112,7 +14116,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <f t="shared" si="5"/>
         <v>385</v>
@@ -14139,7 +14143,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <f t="shared" ref="A388:A451" si="6">A387+1</f>
         <v>386</v>
@@ -14166,7 +14170,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <f t="shared" si="6"/>
         <v>387</v>
@@ -14193,7 +14197,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <f t="shared" si="6"/>
         <v>388</v>
@@ -14220,7 +14224,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <f t="shared" si="6"/>
         <v>389</v>
@@ -14247,7 +14251,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <f t="shared" si="6"/>
         <v>390</v>
@@ -14274,7 +14278,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <f t="shared" si="6"/>
         <v>391</v>
@@ -14301,7 +14305,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <f t="shared" si="6"/>
         <v>392</v>
@@ -14328,7 +14332,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <f t="shared" si="6"/>
         <v>393</v>
@@ -14355,7 +14359,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <f t="shared" si="6"/>
         <v>394</v>
@@ -14382,7 +14386,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <f t="shared" si="6"/>
         <v>395</v>
@@ -14409,7 +14413,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <f t="shared" si="6"/>
         <v>396</v>
@@ -14436,7 +14440,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <f t="shared" si="6"/>
         <v>397</v>
@@ -14463,7 +14467,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <f t="shared" si="6"/>
         <v>398</v>
@@ -14490,7 +14494,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <f t="shared" si="6"/>
         <v>399</v>
@@ -14517,7 +14521,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <f t="shared" si="6"/>
         <v>400</v>
@@ -14544,7 +14548,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <f t="shared" si="6"/>
         <v>401</v>
@@ -14571,7 +14575,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <f t="shared" si="6"/>
         <v>402</v>
@@ -14598,7 +14602,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <f t="shared" si="6"/>
         <v>403</v>
@@ -14625,7 +14629,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <f t="shared" si="6"/>
         <v>404</v>
@@ -14652,7 +14656,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <f t="shared" si="6"/>
         <v>405</v>
@@ -14679,7 +14683,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <f t="shared" si="6"/>
         <v>406</v>
@@ -14706,7 +14710,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <f t="shared" si="6"/>
         <v>407</v>
@@ -14733,7 +14737,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <f t="shared" si="6"/>
         <v>408</v>
@@ -14760,7 +14764,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <f t="shared" si="6"/>
         <v>409</v>
@@ -14787,7 +14791,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <f t="shared" si="6"/>
         <v>410</v>
@@ -14814,7 +14818,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <f t="shared" si="6"/>
         <v>411</v>
@@ -14841,7 +14845,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <f t="shared" si="6"/>
         <v>412</v>
@@ -14868,7 +14872,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <f t="shared" si="6"/>
         <v>413</v>
@@ -14895,7 +14899,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <f t="shared" si="6"/>
         <v>414</v>
@@ -14922,7 +14926,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <f t="shared" si="6"/>
         <v>415</v>
@@ -14949,7 +14953,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <f t="shared" si="6"/>
         <v>416</v>
@@ -14976,7 +14980,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <f t="shared" si="6"/>
         <v>417</v>
@@ -15003,7 +15007,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <f t="shared" si="6"/>
         <v>418</v>
@@ -15030,7 +15034,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <f t="shared" si="6"/>
         <v>419</v>
@@ -15057,7 +15061,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <f t="shared" si="6"/>
         <v>420</v>
@@ -15084,7 +15088,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <f t="shared" si="6"/>
         <v>421</v>
@@ -15111,7 +15115,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <f t="shared" si="6"/>
         <v>422</v>
@@ -15138,7 +15142,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <f t="shared" si="6"/>
         <v>423</v>
@@ -15165,7 +15169,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <f t="shared" si="6"/>
         <v>424</v>
@@ -15192,7 +15196,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <f t="shared" si="6"/>
         <v>425</v>
@@ -15219,7 +15223,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <f t="shared" si="6"/>
         <v>426</v>
@@ -15246,7 +15250,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <f t="shared" si="6"/>
         <v>427</v>
@@ -15273,7 +15277,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <f t="shared" si="6"/>
         <v>428</v>
@@ -15300,7 +15304,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <f t="shared" si="6"/>
         <v>429</v>
@@ -15327,7 +15331,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <f t="shared" si="6"/>
         <v>430</v>
@@ -15354,7 +15358,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <f t="shared" si="6"/>
         <v>431</v>
@@ -15381,7 +15385,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <f t="shared" si="6"/>
         <v>432</v>
@@ -15408,7 +15412,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <f t="shared" si="6"/>
         <v>433</v>
@@ -15435,7 +15439,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <f t="shared" si="6"/>
         <v>434</v>
@@ -15462,7 +15466,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <f t="shared" si="6"/>
         <v>435</v>
@@ -15489,7 +15493,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <f t="shared" si="6"/>
         <v>436</v>
@@ -15516,7 +15520,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <f t="shared" si="6"/>
         <v>437</v>
@@ -15543,7 +15547,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <f t="shared" si="6"/>
         <v>438</v>
@@ -15570,7 +15574,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <f t="shared" si="6"/>
         <v>439</v>
@@ -15597,7 +15601,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <f t="shared" si="6"/>
         <v>440</v>
@@ -15621,7 +15625,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <f t="shared" si="6"/>
         <v>441</v>
@@ -15648,7 +15652,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
         <f t="shared" si="6"/>
         <v>442</v>
@@ -15675,7 +15679,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <f t="shared" si="6"/>
         <v>443</v>
@@ -15702,7 +15706,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <f t="shared" si="6"/>
         <v>444</v>
@@ -15729,7 +15733,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
         <f t="shared" si="6"/>
         <v>445</v>
@@ -15756,7 +15760,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
         <f t="shared" si="6"/>
         <v>446</v>
@@ -15783,7 +15787,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="449" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <f t="shared" si="6"/>
         <v>447</v>
@@ -15810,7 +15814,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="450" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <f t="shared" si="6"/>
         <v>448</v>
@@ -15837,7 +15841,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
         <f t="shared" si="6"/>
         <v>449</v>
@@ -15864,7 +15868,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="452" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
         <f t="shared" ref="A452:A515" si="7">A451+1</f>
         <v>450</v>
@@ -15891,7 +15895,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <f t="shared" si="7"/>
         <v>451</v>
@@ -15918,7 +15922,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="454" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <f t="shared" si="7"/>
         <v>452</v>
@@ -15945,7 +15949,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="455" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <f t="shared" si="7"/>
         <v>453</v>
@@ -15972,7 +15976,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <f t="shared" si="7"/>
         <v>454</v>
@@ -15999,7 +16003,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="457" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <f t="shared" si="7"/>
         <v>455</v>
@@ -16026,7 +16030,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <f t="shared" si="7"/>
         <v>456</v>
@@ -16053,7 +16057,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="459" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <f t="shared" si="7"/>
         <v>457</v>
@@ -16080,7 +16084,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <f t="shared" si="7"/>
         <v>458</v>
@@ -16107,7 +16111,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="461" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <f t="shared" si="7"/>
         <v>459</v>
@@ -16134,7 +16138,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="462" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <f t="shared" si="7"/>
         <v>460</v>
@@ -16161,7 +16165,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <f t="shared" si="7"/>
         <v>461</v>
@@ -16188,7 +16192,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="464" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
         <f t="shared" si="7"/>
         <v>462</v>
@@ -16215,7 +16219,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <f t="shared" si="7"/>
         <v>463</v>
@@ -16242,7 +16246,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <f t="shared" si="7"/>
         <v>464</v>
@@ -16269,7 +16273,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <f t="shared" si="7"/>
         <v>465</v>
@@ -16296,7 +16300,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <f t="shared" si="7"/>
         <v>466</v>
@@ -16323,7 +16327,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
         <f t="shared" si="7"/>
         <v>467</v>
@@ -16350,7 +16354,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="470" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <f t="shared" si="7"/>
         <v>468</v>
@@ -16377,7 +16381,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <f t="shared" si="7"/>
         <v>469</v>
@@ -16404,7 +16408,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <f t="shared" si="7"/>
         <v>470</v>
@@ -16431,7 +16435,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
         <f t="shared" si="7"/>
         <v>471</v>
@@ -16458,7 +16462,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <f t="shared" si="7"/>
         <v>472</v>
@@ -16485,7 +16489,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
         <f t="shared" si="7"/>
         <v>473</v>
@@ -16512,7 +16516,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" s="1">
         <f t="shared" si="7"/>
         <v>474</v>
@@ -16539,7 +16543,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" s="1">
         <f t="shared" si="7"/>
         <v>475</v>
@@ -16566,7 +16570,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="478" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" s="1">
         <f t="shared" si="7"/>
         <v>476</v>
@@ -16593,7 +16597,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="479" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" s="1">
         <f t="shared" si="7"/>
         <v>477</v>
@@ -16620,7 +16624,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" s="1">
         <f t="shared" si="7"/>
         <v>478</v>
@@ -16647,7 +16651,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="481" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" s="1">
         <f t="shared" si="7"/>
         <v>479</v>
@@ -16674,7 +16678,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="482" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" s="1">
         <f t="shared" si="7"/>
         <v>480</v>
@@ -16701,7 +16705,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" s="1">
         <f t="shared" si="7"/>
         <v>481</v>
@@ -16728,7 +16732,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="484" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" s="1">
         <f t="shared" si="7"/>
         <v>482</v>
@@ -16755,7 +16759,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="485" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" s="1">
         <f t="shared" si="7"/>
         <v>483</v>
@@ -16782,7 +16786,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="486" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" s="1">
         <f t="shared" si="7"/>
         <v>484</v>
@@ -16809,7 +16813,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="487" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" s="1">
         <f t="shared" si="7"/>
         <v>485</v>
@@ -16836,7 +16840,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="488" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" s="1">
         <f t="shared" si="7"/>
         <v>486</v>
@@ -16863,7 +16867,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="489" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" s="1">
         <f t="shared" si="7"/>
         <v>487</v>
@@ -16890,7 +16894,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="490" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" s="1">
         <f t="shared" si="7"/>
         <v>488</v>
@@ -16917,7 +16921,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="491" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" s="1">
         <f t="shared" si="7"/>
         <v>489</v>
@@ -16944,7 +16948,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="492" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" s="1">
         <f t="shared" si="7"/>
         <v>490</v>
@@ -16971,7 +16975,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="493" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" s="1">
         <f t="shared" si="7"/>
         <v>491</v>
@@ -16998,7 +17002,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="494" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" s="1">
         <f t="shared" si="7"/>
         <v>492</v>
@@ -17025,7 +17029,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="495" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" s="1">
         <f t="shared" si="7"/>
         <v>493</v>
@@ -17052,7 +17056,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="496" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" s="1">
         <f t="shared" si="7"/>
         <v>494</v>
@@ -17079,7 +17083,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" s="1">
         <f t="shared" si="7"/>
         <v>495</v>
@@ -17106,7 +17110,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" s="1">
         <f t="shared" si="7"/>
         <v>496</v>
@@ -17133,7 +17137,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" s="1">
         <f t="shared" si="7"/>
         <v>497</v>
@@ -17160,7 +17164,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="500" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" s="1">
         <f t="shared" si="7"/>
         <v>498</v>
@@ -17187,7 +17191,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" s="1">
         <f t="shared" si="7"/>
         <v>499</v>
@@ -17214,7 +17218,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" s="1">
         <f t="shared" si="7"/>
         <v>500</v>
@@ -17241,7 +17245,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="503" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" s="1">
         <f t="shared" si="7"/>
         <v>501</v>
@@ -17268,7 +17272,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" s="1">
         <f t="shared" si="7"/>
         <v>502</v>
@@ -17295,7 +17299,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" s="1">
         <f t="shared" si="7"/>
         <v>503</v>
@@ -17322,7 +17326,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="506" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" s="1">
         <f t="shared" si="7"/>
         <v>504</v>
@@ -17349,7 +17353,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" s="1">
         <f t="shared" si="7"/>
         <v>505</v>
@@ -17376,7 +17380,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" s="1">
         <f t="shared" si="7"/>
         <v>506</v>
@@ -17403,7 +17407,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509" s="1">
         <f t="shared" si="7"/>
         <v>507</v>
@@ -17430,7 +17434,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="510" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" s="1">
         <f t="shared" si="7"/>
         <v>508</v>
@@ -17457,7 +17461,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="511" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" s="1">
         <f t="shared" si="7"/>
         <v>509</v>
@@ -17484,7 +17488,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="512" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" s="1">
         <f t="shared" si="7"/>
         <v>510</v>
@@ -17511,7 +17515,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" s="1">
         <f t="shared" si="7"/>
         <v>511</v>
@@ -17538,7 +17542,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="514" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" s="1">
         <f t="shared" si="7"/>
         <v>512</v>
@@ -17565,7 +17569,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="515" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A515" s="1">
         <f t="shared" si="7"/>
         <v>513</v>
@@ -17592,7 +17596,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A516" s="1">
         <f t="shared" ref="A516:A523" si="8">A515+1</f>
         <v>514</v>
@@ -17619,7 +17623,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="517" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" s="1">
         <f t="shared" si="8"/>
         <v>515</v>
@@ -17646,7 +17650,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" s="1">
         <f t="shared" si="8"/>
         <v>516</v>
@@ -17673,7 +17677,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519" s="1">
         <f t="shared" si="8"/>
         <v>517</v>
@@ -17700,7 +17704,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520" s="1">
         <f t="shared" si="8"/>
         <v>518</v>
@@ -17727,7 +17731,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="521" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" s="1">
         <f t="shared" si="8"/>
         <v>519</v>
@@ -17754,7 +17758,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="522" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" s="1">
         <f t="shared" si="8"/>
         <v>520</v>
@@ -17781,7 +17785,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="523" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" s="1">
         <f t="shared" si="8"/>
         <v>521</v>
@@ -17809,6 +17813,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G523" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Sistemas de óleo lubrificante"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>